<commit_message>
added testcases to email services api
</commit_message>
<xml_diff>
--- a/src/test/test-data/EmailServiceTestData.xlsx
+++ b/src/test/test-data/EmailServiceTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS00465091\git\1p-api-automation\src\test\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -164,9 +164,6 @@
     <t>status=200||userid=(OPQA-5865_userid)||email=(OPQA-5865_email)||provider=verified_email</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>status=200||provider=st||email=(OPQA-5865_email)</t>
   </si>
   <si>
@@ -182,7 +179,400 @@
     <t>/email/steam/primary</t>
   </si>
   <si>
-    <t>{"userid": "(OPQA-5865_userid)","email": "updated(OPQA-5865_email)","previousEmail":"(OPAQ-5865_email)"}</t>
+    <t>OPQA-5876</t>
+  </si>
+  <si>
+    <t>Verifying that user  is able to returns primary emails for given list of userids</t>
+  </si>
+  <si>
+    <t>/email/platform/primary/batch/cmty</t>
+  </si>
+  <si>
+    <t>["(OPQA-5865_userid)", "(OPQA-5865_1_userid)"]</t>
+  </si>
+  <si>
+    <t>OPQA-5877</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get error message for given list of invalid userid</t>
+  </si>
+  <si>
+    <t>status=500</t>
+  </si>
+  <si>
+    <t>["(OPQA-5865_userid)11"]</t>
+  </si>
+  <si>
+    <t>{"userid": "(OPQA-5865_userid)","email": "updateduser+(ddMMMyyyy_HHmmss)@gmail.com","previousEmail":"(OPQA-5865_email)"}</t>
+  </si>
+  <si>
+    <t>status=200||count=2||emails.userid[0]=(OPQA-5865_userid)||emails.userid[1]=(OPQA-5865_1_userid)</t>
+  </si>
+  <si>
+    <t>status=400</t>
+  </si>
+  <si>
+    <t>OPQA-5878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the error message if we pass list of userid more than 100 </t>
+  </si>
+  <si>
+    <t>["2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5"]</t>
+  </si>
+  <si>
+    <t>OPQA-5879</t>
+  </si>
+  <si>
+    <t>verify that api email api returns list of user ids and emails for given list of verified emails</t>
+  </si>
+  <si>
+    <t>/email/platform/user/batch/cmty</t>
+  </si>
+  <si>
+    <t>["(OPQA-5865_1_email)","(OPQA-5872_email)"]</t>
+  </si>
+  <si>
+    <t>status=200||count=2||emails.email[0]=(OPQA-5865_1_email)||emails.email[1]=(OPQA-5872_email)</t>
+  </si>
+  <si>
+    <t>OPQA-5880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the error message if we pass list of usersemails  more than 100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">["emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com",
+"emailldemo11@test.com"]
+</t>
+  </si>
+  <si>
+    <t>OPQA-5882</t>
+  </si>
+  <si>
+    <t>Verify that  user is able to return all emails (verified and unverified) for given list of userids.</t>
+  </si>
+  <si>
+    <t>/email/platform/useremails/batch/cmty</t>
+  </si>
+  <si>
+    <t>status=200</t>
+  </si>
+  <si>
+    <t>email||userid</t>
+  </si>
+  <si>
+    <t>["(OPQA-5865_1_userid)", "(OPQA-5872_userid)"]</t>
+  </si>
+  <si>
+    <t>["2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5",
+"2131cbb0-cb94-11e8-9042-617b05c8aed5"]</t>
+  </si>
+  <si>
+    <t>OPQA-5883</t>
+  </si>
+  <si>
+    <t>Verify that status code if we pass invalid emais</t>
   </si>
 </sst>
 </file>
@@ -274,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -298,6 +688,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,22 +996,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="69.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29.140625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="85.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="62.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="57.140625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1" collapsed="1"/>
   </cols>
@@ -691,9 +1084,6 @@
       <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -725,9 +1115,6 @@
         <v>25</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -759,9 +1146,6 @@
         <v>20</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -792,9 +1176,6 @@
       </c>
       <c r="K5" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="L5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -822,12 +1203,9 @@
         <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -857,9 +1235,6 @@
         <v>38</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="L7" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -889,9 +1264,6 @@
         <v>42</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -921,22 +1293,19 @@
         <v>46</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>27</v>
@@ -946,15 +1315,226 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="2"/>
+      <c r="C11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new test case to email api
</commit_message>
<xml_diff>
--- a/src/test/test-data/EmailServiceTestData.xlsx
+++ b/src/test/test-data/EmailServiceTestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -573,6 +573,12 @@
   </si>
   <si>
     <t>Verify that status code if we pass invalid emais</t>
+  </si>
+  <si>
+    <t>OPQA-5881</t>
+  </si>
+  <si>
+    <t>Verify that status code if we pass empty  data in the request</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L20"/>
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,30 +1517,57 @@
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>